<commit_message>
add evidence to B1~B6
</commit_message>
<xml_diff>
--- a/marryton007/evidence.xlsx
+++ b/marryton007/evidence.xlsx
@@ -32,13 +32,14 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="94">
   <si>
     <t>TeamName</t>
   </si>
@@ -304,10 +305,22 @@
     <t>315418CF6299F4E2F2FBBD0F3804041B0993754C2D6A82D0AEEC5B151B7D7E4D</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
-    <t>The Internal Transfer TxHash on IRISnet</t>
+    <t>19680C762BF4B581EC9BC45E2AD3CEFC6713E0BE7D6C75A73A2360DAE144F41E</t>
+  </si>
+  <si>
+    <t>D4D24BBE5D0FC4554F8DDC455D2D5C2E19D801A7B3DBE77D1185B6C6085C662F</t>
+  </si>
+  <si>
+    <t>2015195D628E78D1709DB59A530ED4A27262A617996891516A95C2DB787F8C39</t>
+  </si>
+  <si>
+    <t>24E99CA3ABC00B6C77D4B1CA314EED1BE5140F7256B51B5ABBBDF8A64504255A</t>
+  </si>
+  <si>
+    <t>F7137C060DABAC746C84A289067904FE76C630B3752DFFEA9660423D1B9CB8DD</t>
+  </si>
+  <si>
+    <t>845EF268B95B1585F009036154C549562F60828333D476F34B206AC08E1347FE</t>
   </si>
 </sst>
 </file>
@@ -315,9 +328,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -348,57 +361,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -410,15 +376,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -439,17 +397,11 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -461,8 +413,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -477,15 +461,44 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -506,61 +519,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -572,121 +699,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -718,6 +731,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -733,37 +757,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -784,161 +788,170 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2164,7 +2177,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5714285714286" defaultRowHeight="12" outlineLevelRow="2"/>
@@ -2203,7 +2216,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5714285714286" defaultRowHeight="12" outlineLevelRow="2"/>
@@ -2239,7 +2252,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5714285714286" defaultRowHeight="12" outlineLevelRow="2"/>
@@ -2251,12 +2264,12 @@
     </row>
     <row r="2" ht="13.2" spans="1:1">
       <c r="A2" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" ht="13.2" spans="1:1">
       <c r="A3" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2266,6 +2279,39 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelRow="2"/>
+  <sheetData>
+    <row r="1" ht="13.2" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 

</xml_diff>